<commit_message>
add one more file to checkout
</commit_message>
<xml_diff>
--- a/results/ul-east-1/ALL-results-ul-east-1.xlsx
+++ b/results/ul-east-1/ALL-results-ul-east-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Google Drive/serverlessComputingProject/7x24/results/ul-east-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54419D4-A326-1A48-A87B-2A3DE95E86A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0AA0DA-836A-764E-B3BE-AFB3C27C242B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{F749A59E-DDC3-734D-AD3F-AC79494060BD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21900" xr2:uid="{F749A59E-DDC3-734D-AD3F-AC79494060BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Upper Boun</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>cold/warm starts</t>
+  </si>
+  <si>
+    <t>HERE</t>
   </si>
 </sst>
 </file>
@@ -397,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F732CCB1-47D2-074D-981F-B1B82B5AA75F}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,6 +621,9 @@
       <c r="I8">
         <v>9</v>
       </c>
+      <c r="V8" t="s">
+        <v>3</v>
+      </c>
       <c r="AF8">
         <v>360</v>
       </c>
@@ -626,6 +632,9 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="V9" t="s">
+        <v>3</v>
+      </c>
       <c r="AF9">
         <v>300</v>
       </c>

</xml_diff>